<commit_message>
Created Geographic English Group and Started on Geographic Thai Group. Added buttons to switch language. And added Image Visual for Background not used Canvas Background as with an Image I can Change the image used as the background when I use a bookmark. It wil need testing to see what the performance like as I'm going to have a lot of visuals on the one page.
</commit_message>
<xml_diff>
--- a/Data/BiLingual Text Strings.xlsx
+++ b/Data/BiLingual Text Strings.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/efcfa07183130be2/Documents/001 - Power BI ^0 Data Visualisation/In Development/Active/EEC Factory Analysis - Power BI Version/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="8_{C9F57D40-F516-4FD4-9725-FDAEE5B23993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83F748D7-F282-4861-90AB-9BB7EB05F5F7}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{C9F57D40-F516-4FD4-9725-FDAEE5B23993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3B9C6B0-68A9-48FC-9377-E1DA97C9CFFC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" activeTab="1" xr2:uid="{E82FD87B-5AA0-43B2-87CE-B1C55C908D64}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" xr2:uid="{E82FD87B-5AA0-43B2-87CE-B1C55C908D64}"/>
   </bookViews>
   <sheets>
     <sheet name="Report Titles" sheetId="1" r:id="rId1"/>
-    <sheet name="Selected Province" sheetId="3" r:id="rId2"/>
-    <sheet name="Geo Analysis Buttons" sheetId="2" r:id="rId3"/>
+    <sheet name="Geo Analysis Buttons" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Language_Selected">'Geo Analysis Buttons'!$B$1</definedName>
@@ -86,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="188">
   <si>
     <t>Analysis Type</t>
   </si>
@@ -163,18 +162,6 @@
     <t>จังหวัดตามพื้นที่อาคาร (ตร.มล.)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Province  by Building Value (M. Baht)</t>
-  </si>
-  <si>
-    <t>จังหวัดตามมูลค่าอาคาร (ล้านบาท)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> District by No. of Factories</t>
-  </si>
-  <si>
-    <t>อำเภอตามจำนวนโรงงาน</t>
-  </si>
-  <si>
     <t>Total No. of Factories</t>
   </si>
   <si>
@@ -239,12 +226,6 @@
   </si>
   <si>
     <t>รหัสไปรษณีย์ ตามพื้นที่อาคาร (ตร.ม.)</t>
-  </si>
-  <si>
-    <t>Postcode by Building Value (Baht)</t>
-  </si>
-  <si>
-    <t>รหัสไปรษณีย์ ตามมูลค่าอาคาร (บาท)</t>
   </si>
   <si>
     <t>Top 10 Districts by No. of Factories</t>
@@ -589,15 +570,6 @@
     <t>Geo_Province_Chart_Title</t>
   </si>
   <si>
-    <t>Geo_District_Chart_Title</t>
-  </si>
-  <si>
-    <t>Geo_Top 10 Sub District Chart Title</t>
-  </si>
-  <si>
-    <t>Geo_Postcode Chart Title</t>
-  </si>
-  <si>
     <t>Geo_Top_10_District_Chart_Title</t>
   </si>
   <si>
@@ -607,9 +579,6 @@
     <t>Inv_Total_Card_Title</t>
   </si>
   <si>
-    <t>Inv_Postcode Chart Title</t>
-  </si>
-  <si>
     <t>Inv_District_Chart_Title</t>
   </si>
   <si>
@@ -646,9 +615,6 @@
     <t>Ind_Group_Analysis_Title</t>
   </si>
   <si>
-    <t>Ind_Group Total Investment Title</t>
-  </si>
-  <si>
     <t>Entity</t>
   </si>
   <si>
@@ -688,34 +654,16 @@
     <t>Geo_Total_Card_Title</t>
   </si>
   <si>
-    <t>province code</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>ชลบุรี</t>
-  </si>
-  <si>
-    <t>Chonburi</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>ระยอง</t>
-  </si>
-  <si>
-    <t>Rayong</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>ฉะเชิงเทรา</t>
-  </si>
-  <si>
-    <t>Chachoengsao</t>
+    <t>Inv_Postcode_Chart_Title</t>
+  </si>
+  <si>
+    <t>Geo_Top_10_Sub_District_Chart_Title</t>
+  </si>
+  <si>
+    <t>Ind_Group_Total_Investment_Title</t>
+  </si>
+  <si>
+    <t>Geo_Postcode_Chart_Title</t>
   </si>
 </sst>
 </file>
@@ -761,7 +709,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -793,14 +741,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -808,11 +851,99 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="11">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -890,12 +1021,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}" name="Table1" displayName="Table1" ref="A1:D87" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="A1:D87" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}" name="Table1" displayName="Table1" ref="A1:D84" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="A1:D84" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{EA6343D5-1FE2-43FC-991F-9F660BDA0B22}" name="Entity"/>
     <tableColumn id="2" xr3:uid="{8B2E6FF6-2773-4399-9327-594910EEDC92}" name="Analysis Type"/>
-    <tableColumn id="3" xr3:uid="{23066573-0C1B-4965-95E7-7C81C836CD35}" name="English" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{23066573-0C1B-4965-95E7-7C81C836CD35}" name="English" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{58EB589B-59BD-4A1B-ACBA-F3BFBFDC54C5}" name="ภาษาไทย"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -903,12 +1034,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{87F671DB-53E0-477F-A0FE-AF69F685FC1B}" name="Table2" displayName="Table2" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{87F671DB-53E0-477F-A0FE-AF69F685FC1B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{316CFFA1-5176-4B66-A6A6-0F3B9A1CEC03}" name="Table2" displayName="Table2" ref="A1:C4" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C4" xr:uid="{316CFFA1-5176-4B66-A6A6-0F3B9A1CEC03}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4724FBF3-FE04-40C6-A122-18AF28520863}" name="province code"/>
-    <tableColumn id="2" xr3:uid="{A625C562-8A90-4879-9944-ADAE4CF7E9C9}" name="ภาษาไทย"/>
-    <tableColumn id="3" xr3:uid="{6B12BC19-B235-4557-927F-F58464239467}" name="English"/>
+    <tableColumn id="1" xr3:uid="{828FEEFC-73D2-498D-858C-6869171D8DFD}" name="Analysis_Type" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{5343A523-A207-4019-B160-7FABD2911CFD}" name="English" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{F4E06540-8FBF-43CA-833B-3190AFDB460B}" name="ภาษาไทย" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1229,42 +1360,42 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B33C440-B339-49E7-80B6-40EB80459ED5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.6640625" customWidth="1"/>
     <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="51.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>153</v>
+      <c r="C1" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
@@ -1273,12 +1404,12 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
@@ -1287,12 +1418,12 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
@@ -1301,12 +1432,12 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
@@ -1315,12 +1446,12 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
@@ -1329,26 +1460,26 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>190</v>
+      <c r="C7" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="D7" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
@@ -1357,12 +1488,12 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="s">
@@ -1376,7 +1507,7 @@
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
@@ -1390,7 +1521,7 @@
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D11" t="s">
@@ -1399,12 +1530,12 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
@@ -1413,12 +1544,12 @@
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D13" t="s">
@@ -1427,26 +1558,26 @@
     </row>
     <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D15" t="s">
@@ -1455,12 +1586,12 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D16" t="s">
@@ -1469,54 +1600,54 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19">
         <v>2</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>194</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>33</v>
+      <c r="C19" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D20" t="s">
@@ -1525,40 +1656,40 @@
     </row>
     <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="B22">
-        <v>3</v>
-      </c>
-      <c r="C22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="C23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D23" t="s">
@@ -1567,138 +1698,138 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>156</v>
+      </c>
+      <c r="B26">
         <v>2</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C26" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>164</v>
-      </c>
-      <c r="B26">
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27">
         <v>3</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C27" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>164</v>
-      </c>
-      <c r="B27">
-        <v>4</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="D27" t="s">
         <v>51</v>
-      </c>
-      <c r="D27" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29">
         <v>1</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>165</v>
-      </c>
-      <c r="B29">
+      <c r="C29" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30">
         <v>2</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>165</v>
-      </c>
-      <c r="B30">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31">
         <v>3</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>165</v>
-      </c>
-      <c r="B31">
-        <v>4</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>35</v>
+        <v>4</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="D32" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B33">
-        <v>2</v>
-      </c>
-      <c r="C33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D33" t="s">
@@ -1707,82 +1838,82 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B34">
-        <v>3</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>62</v>
+        <v>1</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B35">
-        <v>4</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>64</v>
+        <v>2</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B36">
-        <v>5</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>66</v>
+        <v>3</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="D36" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>35</v>
+        <v>4</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B38">
-        <v>2</v>
-      </c>
-      <c r="C38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D38" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="B39">
-        <v>3</v>
-      </c>
-      <c r="C39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D39" t="s">
@@ -1791,124 +1922,124 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="B40">
-        <v>4</v>
-      </c>
-      <c r="C40" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D40" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="B41">
-        <v>5</v>
-      </c>
-      <c r="C41" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" t="s">
         <v>66</v>
       </c>
-      <c r="D41" t="s">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>184</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>168</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" s="5" t="s">
+      <c r="D42" t="s">
         <v>68</v>
-      </c>
-      <c r="D42" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45">
         <v>2</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>168</v>
-      </c>
-      <c r="B44">
+      <c r="C45" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>159</v>
+      </c>
+      <c r="B46">
         <v>3</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>168</v>
-      </c>
-      <c r="B45">
-        <v>4</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="C46" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>168</v>
-      </c>
-      <c r="B46">
-        <v>5</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D46" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>58</v>
+        <v>4</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="D47" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B48">
-        <v>2</v>
-      </c>
-      <c r="C48" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D48" t="s">
@@ -1917,55 +2048,55 @@
     </row>
     <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B49">
-        <v>3</v>
-      </c>
-      <c r="C49" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" t="s">
         <v>79</v>
-      </c>
-      <c r="D49" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B50">
-        <v>4</v>
-      </c>
-      <c r="C50" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" t="s">
         <v>81</v>
-      </c>
-      <c r="D50" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B51">
-        <v>5</v>
-      </c>
-      <c r="C51" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" t="s">
         <v>83</v>
-      </c>
-      <c r="D51" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>43</v>
+        <v>4</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="D52" t="s">
         <v>85</v>
@@ -1973,54 +2104,54 @@
     </row>
     <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B53">
-        <v>2</v>
-      </c>
-      <c r="C53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>86</v>
       </c>
       <c r="D53" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B54">
-        <v>3</v>
-      </c>
-      <c r="C54" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D54" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B55">
-        <v>4</v>
-      </c>
-      <c r="C55" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>90</v>
       </c>
       <c r="D55" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B56">
-        <v>5</v>
-      </c>
-      <c r="C56" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>92</v>
       </c>
       <c r="D56" t="s">
@@ -2029,54 +2160,54 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>94</v>
+      <c r="C57" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="D57" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B58">
         <v>2</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>96</v>
+      <c r="C58" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="D58" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B59">
         <v>3</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>98</v>
+      <c r="C59" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="D59" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D60" t="s">
@@ -2085,12 +2216,12 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B61">
         <v>2</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="4" t="s">
         <v>96</v>
       </c>
       <c r="D61" t="s">
@@ -2099,12 +2230,12 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B62">
         <v>3</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="4" t="s">
         <v>98</v>
       </c>
       <c r="D62" t="s">
@@ -2113,12 +2244,12 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="4" t="s">
         <v>100</v>
       </c>
       <c r="D63" t="s">
@@ -2127,54 +2258,54 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B64">
         <v>2</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="4" t="s">
         <v>102</v>
       </c>
       <c r="D64" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B65">
         <v>3</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D65" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="4" t="s">
         <v>106</v>
       </c>
       <c r="D66" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B67">
         <v>2</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="4" t="s">
         <v>108</v>
       </c>
       <c r="D67" t="s">
@@ -2183,96 +2314,96 @@
     </row>
     <row r="68" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B68">
         <v>3</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="4" t="s">
         <v>110</v>
       </c>
       <c r="D68" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>112</v>
       </c>
       <c r="D69" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B70">
-        <v>2</v>
-      </c>
-      <c r="C70" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>114</v>
       </c>
       <c r="D70" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B71">
-        <v>3</v>
-      </c>
-      <c r="C71" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>116</v>
       </c>
       <c r="D71" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B72">
-        <v>0</v>
-      </c>
-      <c r="C72" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>118</v>
       </c>
       <c r="D72" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B73">
-        <v>0</v>
-      </c>
-      <c r="C73" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>120</v>
       </c>
       <c r="D73" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B74">
-        <v>0</v>
-      </c>
-      <c r="C74" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>122</v>
       </c>
       <c r="D74" t="s">
@@ -2281,12 +2412,12 @@
     </row>
     <row r="75" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B75">
-        <v>1</v>
-      </c>
-      <c r="C75" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D75" t="s">
@@ -2295,12 +2426,12 @@
     </row>
     <row r="76" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B76">
-        <v>2</v>
-      </c>
-      <c r="C76" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="4" t="s">
         <v>126</v>
       </c>
       <c r="D76" t="s">
@@ -2309,12 +2440,12 @@
     </row>
     <row r="77" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B77">
-        <v>3</v>
-      </c>
-      <c r="C77" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>128</v>
       </c>
       <c r="D77" t="s">
@@ -2323,12 +2454,12 @@
     </row>
     <row r="78" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B78">
-        <v>4</v>
-      </c>
-      <c r="C78" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>130</v>
       </c>
       <c r="D78" t="s">
@@ -2337,12 +2468,12 @@
     </row>
     <row r="79" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B79">
-        <v>5</v>
-      </c>
-      <c r="C79" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79" s="4" t="s">
         <v>132</v>
       </c>
       <c r="D79" t="s">
@@ -2351,26 +2482,26 @@
     </row>
     <row r="80" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B80">
-        <v>1</v>
-      </c>
-      <c r="C80" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>134</v>
       </c>
       <c r="D80" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B81">
-        <v>2</v>
-      </c>
-      <c r="C81" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>136</v>
       </c>
       <c r="D81" t="s">
@@ -2379,86 +2510,44 @@
     </row>
     <row r="82" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B82">
-        <v>3</v>
-      </c>
-      <c r="C82" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D82" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="B83">
-        <v>4</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>140</v>
+        <v>0</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="D83" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
       <c r="B84">
-        <v>5</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D84" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>181</v>
-      </c>
-      <c r="B85">
         <v>0</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C84" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D84" s="4" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>146</v>
-      </c>
-      <c r="B86">
-        <v>0</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="D86" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>149</v>
-      </c>
-      <c r="B87">
-        <v>0</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2472,62 +2561,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36E7C13-408F-481B-B585-420319E379F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732BE711-A846-4BDE-A432-7EBD4B1436D1}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" t="s">
-        <v>152</v>
+      <c r="A1" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2" t="s">
-        <v>198</v>
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>199</v>
-      </c>
-      <c r="B3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C3" t="s">
-        <v>201</v>
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>202</v>
-      </c>
-      <c r="B4" t="s">
-        <v>203</v>
-      </c>
-      <c r="C4" t="s">
-        <v>204</v>
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2536,66 +2625,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732BE711-A846-4BDE-A432-7EBD4B1436D1}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Dashboards, For Geographic, Invesment & Workforce completed. Remaining are Industry, Address List and Information
</commit_message>
<xml_diff>
--- a/Data/BiLingual Text Strings.xlsx
+++ b/Data/BiLingual Text Strings.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/efcfa07183130be2/Documents/001 - Power BI ^0 Data Visualisation/In Development/Active/EEC Factory Analysis - Power BI Version/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{C9F57D40-F516-4FD4-9725-FDAEE5B23993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3B9C6B0-68A9-48FC-9377-E1DA97C9CFFC}"/>
+  <xr:revisionPtr revIDLastSave="313" documentId="8_{C9F57D40-F516-4FD4-9725-FDAEE5B23993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A259D03-D07D-4AFA-9A91-669F365805B0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" xr2:uid="{E82FD87B-5AA0-43B2-87CE-B1C55C908D64}"/>
   </bookViews>
   <sheets>
     <sheet name="Report Titles" sheetId="1" r:id="rId1"/>
-    <sheet name="Geo Analysis Buttons" sheetId="2" r:id="rId2"/>
+    <sheet name="Wkf Analysis Buttons" sheetId="4" r:id="rId2"/>
+    <sheet name="Ind Analysis Buttons" sheetId="5" r:id="rId3"/>
+    <sheet name="Geo Analysis Buttons" sheetId="2" r:id="rId4"/>
+    <sheet name="Inv Analysis Buttons" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="Language_Selected">'Geo Analysis Buttons'!$B$1</definedName>
+    <definedName name="Language_Selected">'Ind Analysis Buttons'!$B$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -85,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="221">
   <si>
     <t>Analysis Type</t>
   </si>
@@ -147,21 +150,12 @@
     <t xml:space="preserve"> Province by No. of Factories</t>
   </si>
   <si>
-    <t>จังหวัดที่ไม่มีโรงงาน</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Province by Factory Area (Sq M m.)</t>
   </si>
   <si>
-    <t>จังหวัดแบ่งตามพื้นที่โรงงาน (ตร.มล.)</t>
-  </si>
-  <si>
     <t>Province by Building Area (Sq M m.)</t>
   </si>
   <si>
-    <t>จังหวัดตามพื้นที่อาคาร (ตร.มล.)</t>
-  </si>
-  <si>
     <t>Total No. of Factories</t>
   </si>
   <si>
@@ -189,84 +183,24 @@
     <t>Top 10 Sub-Districts by No. of Factories</t>
   </si>
   <si>
-    <t>10 อันดับตำบลเรียงตามจำนวนโรงงาน</t>
-  </si>
-  <si>
-    <t>Top 10 Sub-Districts by Factory Area (Sq m.)</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบลแยกตามพื้นที่โรงงาน</t>
-  </si>
-  <si>
-    <t>Top 10 Sub-Districts by Building Area (Sq m.)</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบล แยกตามพื้นที่อาคาร (ตร.ม.)</t>
-  </si>
-  <si>
     <t>Top 10 Sub-Districts by Building Value (M. Baht)</t>
   </si>
   <si>
-    <t>10 อันดับตำบล แยกตามมูลค่าอาคาร (ล้านบาท)</t>
-  </si>
-  <si>
     <t>Postcode by No. of Factories</t>
   </si>
   <si>
-    <t>รหัสไปรษณีย์ตามจำนวนโรงงาน</t>
-  </si>
-  <si>
-    <t>Postcode by Factory Area (Sq m.)</t>
-  </si>
-  <si>
-    <t>รหัสไปรษณีย์ ตามพื้นที่โรงงาน (ตร.ม.)</t>
-  </si>
-  <si>
-    <t>Postcode by Building Area (Sq m.)</t>
-  </si>
-  <si>
-    <t>รหัสไปรษณีย์ ตามพื้นที่อาคาร (ตร.ม.)</t>
-  </si>
-  <si>
     <t>Top 10 Districts by No. of Factories</t>
   </si>
   <si>
-    <t>Top 10 Districts by Factory Area (Sq m.)</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอแบ่งตามพื้นที่โรงงาน (ตร.ม.)</t>
-  </si>
-  <si>
-    <t>Top 10 Districts by Building Area (Sq m.)</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอแบ่งตามพื้นที่อาคาร (ตร.ม.)</t>
-  </si>
-  <si>
     <t>Top 10 Districts by Building Value (M. Baht)</t>
   </si>
   <si>
-    <t>10 อันดับอำเภอ เรียงตามมูลค่าอาคาร (ล้านบาท)</t>
-  </si>
-  <si>
     <t>Total Land Value (M. Baht)</t>
   </si>
   <si>
     <t>มูลค่าที่ดินรวม (ล้านบาท)</t>
   </si>
   <si>
-    <t>Total Machine Cost</t>
-  </si>
-  <si>
-    <t>ค่าเครื่องจักรทั้งหมด</t>
-  </si>
-  <si>
-    <t>Total Working Capital</t>
-  </si>
-  <si>
-    <t>เงินทุนหมุนเวียนทั้งหมด</t>
-  </si>
-  <si>
     <t>Total Investment</t>
   </si>
   <si>
@@ -276,81 +210,39 @@
     <t>Postcode by Building Value (M. Baht)</t>
   </si>
   <si>
-    <t>รหัสไปรษณีย์ ตามมูลค่าอาคาร (ล้านบาท)</t>
-  </si>
-  <si>
     <t>Postcode by Land Value (M. Baht)</t>
   </si>
   <si>
-    <t>Postcode by Machine Cost</t>
-  </si>
-  <si>
-    <t>รหัสไปรษณีย์ตามต้นทุนของเครื่องจักร</t>
-  </si>
-  <si>
     <t>Postcode by Working Capital</t>
   </si>
   <si>
-    <t>รหัสไปรษณีย์ตามเงินทุนหมุนเวียน</t>
-  </si>
-  <si>
     <t>Postcode by Total Investment</t>
   </si>
   <si>
-    <t>รหัสไปรษณีย์ตามการลงทุนทั้งหมด</t>
-  </si>
-  <si>
     <t>Top 10 Districts by Land Value (M. Baht)</t>
   </si>
   <si>
-    <t>10 อันดับอำเภอ จำแนกตามมูลค่าที่ดิน (ล้านบาท)</t>
-  </si>
-  <si>
     <t>Top 10 Districts by Machine Cost (M. Baht)</t>
   </si>
   <si>
-    <t>10 อันดับสูงสุด อำเภอ ตามราคาเครื่อง (ล้านบาท)</t>
-  </si>
-  <si>
     <t>Top 10 Districts by Working Capital (M. Baht)</t>
   </si>
   <si>
-    <t>10 อันดับแรก แยกตามเงินทุนหมุนเวียน (ล้านบาท)</t>
-  </si>
-  <si>
     <t>Top 10 Districts by Total Investment (M. Baht)</t>
   </si>
   <si>
-    <t>10 อันดับอำเภอตามการลงทุนรวม (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบล เรียงตามมูลค่าอาคาร (ล้านบาท)</t>
-  </si>
-  <si>
     <t>Top 10 Sub-Districts by Land Value (M. Baht)</t>
   </si>
   <si>
-    <t>10 อันดับตำบล จำแนกตามมูลค่าที่ดิน (ล้านบาท)</t>
-  </si>
-  <si>
     <t>Top 10 Sub-Districts by Machine Cost (M. Baht)</t>
   </si>
   <si>
-    <t>10 อันดับตำบล จำแนกตามราคาเครื่องจักร (ล้านบาท)</t>
-  </si>
-  <si>
     <t>Top 10 Sub-Districts by Working Capital (M. Baht)</t>
   </si>
   <si>
-    <t>10 อันดับตำบล แยกตามเงินทุนหมุนเวียน (ล้านบาท)</t>
-  </si>
-  <si>
     <t>Top 10 Sub-Districts by Total Investment (M. Baht)</t>
   </si>
   <si>
-    <t>10 อันดับตำบล ตามมูลค่าการลงทุนรวม (ล้านบาท)</t>
-  </si>
-  <si>
     <t>Total Workers</t>
   </si>
   <si>
@@ -390,39 +282,21 @@
     <t>Top 10 Districts by Total Workers</t>
   </si>
   <si>
-    <t>10 อันดับแรกของเขตโดยคนงานทั้งหมด</t>
-  </si>
-  <si>
     <t>Top 10 Districts by Male Workers</t>
   </si>
   <si>
-    <t>10 อันดับแรกของอำเภอโดยคนงานชาย</t>
-  </si>
-  <si>
     <t>Top 10 Districts by Female Workers</t>
   </si>
   <si>
-    <t>10 อันดับแรกของอำเภอโดยคนงานหญิง</t>
-  </si>
-  <si>
     <t>Top 10 Sub-Districts by Total Workers</t>
   </si>
   <si>
-    <t>10 อันดับแรกของตำบลโดยคนงานทั้งหมด</t>
-  </si>
-  <si>
     <t>Top 10 Sub-Districts by Male Workers</t>
   </si>
   <si>
-    <t>10 อันดับแรกของตำบลโดยคนงานชาย</t>
-  </si>
-  <si>
     <t>Top 10 Sub-Districts by Female Workers</t>
   </si>
   <si>
-    <t>10 อันดับแรกของตำบลโดยคนงานหญิง</t>
-  </si>
-  <si>
     <t>Male vs Female Workers</t>
   </si>
   <si>
@@ -474,13 +348,7 @@
     <t>Industry Group by No. of Factories</t>
   </si>
   <si>
-    <t>กลุ่มอุตสาหกรรมแยกตามจำนวนโรงงาน</t>
-  </si>
-  <si>
     <t>Industry Group by Factory Area (sq m.)</t>
-  </si>
-  <si>
-    <t>กลุ่มอุตสาหกรรมแยกตามพื้นที่โรงงาน (ตร.ม.)</t>
   </si>
   <si>
     <t>Industry Group by Building Area (sq m.)</t>
@@ -543,9 +411,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>ภาษาไทย</t>
-  </si>
-  <si>
     <t>Dashboard_Title</t>
   </si>
   <si>
@@ -570,9 +435,6 @@
     <t>Geo_Province_Chart_Title</t>
   </si>
   <si>
-    <t>Geo_Top_10_District_Chart_Title</t>
-  </si>
-  <si>
     <t>Inv_Province_Chart_Title</t>
   </si>
   <si>
@@ -591,9 +453,6 @@
     <t>Wkf_Total_Card_Title</t>
   </si>
   <si>
-    <t>Wkf_Postcode Chart Title</t>
-  </si>
-  <si>
     <t>Wkf_District_Chart_Title</t>
   </si>
   <si>
@@ -648,22 +507,265 @@
     <t>Analysis_Types_Slicer_Title</t>
   </si>
   <si>
-    <t>10 อันดับแรกของอำเภอตามจำนวนโรงงาน</t>
-  </si>
-  <si>
     <t>Geo_Total_Card_Title</t>
   </si>
   <si>
     <t>Inv_Postcode_Chart_Title</t>
   </si>
   <si>
-    <t>Geo_Top_10_Sub_District_Chart_Title</t>
-  </si>
-  <si>
     <t>Ind_Group_Total_Investment_Title</t>
   </si>
   <si>
     <t>Geo_Postcode_Chart_Title</t>
+  </si>
+  <si>
+    <t>Thai</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>Building Value</t>
+  </si>
+  <si>
+    <t>มูลค่าอาคาร</t>
+  </si>
+  <si>
+    <t>Land Value</t>
+  </si>
+  <si>
+    <t>มูลค่าที่ดิน</t>
+  </si>
+  <si>
+    <t>Machine Cost</t>
+  </si>
+  <si>
+    <t>ค่าเครื่อง</t>
+  </si>
+  <si>
+    <t>Working Capital</t>
+  </si>
+  <si>
+    <t>เงินทุนหมุนเวียน</t>
+  </si>
+  <si>
+    <t>Total Machine Cost (M. Baht)</t>
+  </si>
+  <si>
+    <t>ค่าเครื่องจักรทั้งหมด (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>เงินทุนหมุนเวียนทั้งหมด (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>การลงทุนทั้งหมด (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>Total Working Capital (M. Baht)</t>
+  </si>
+  <si>
+    <t>Total Investment (M. Baht)</t>
+  </si>
+  <si>
+    <t>Postcode by Machine Cost (M. Baht)</t>
+  </si>
+  <si>
+    <t>Top 10 Sub-Districts by Factory Area (Sq M m.)</t>
+  </si>
+  <si>
+    <t>Top 10 Districts by Factory Area (Sq M m.)</t>
+  </si>
+  <si>
+    <t>Postcode by Factory Area (Sq M m.)</t>
+  </si>
+  <si>
+    <t>Postcode by Building Area (Sq M m.)</t>
+  </si>
+  <si>
+    <t>Top 10 Sub-Districts by Building Area (Sq M m.)</t>
+  </si>
+  <si>
+    <t>Top 10 Districts by Building Area (Sq M m.)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอแยกตามราคาเครื่อง (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอแยกคนงานทั้งหมด</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอแยกคนงานชาย</t>
+  </si>
+  <si>
+    <t>Province by Building Value (M. Baht)</t>
+  </si>
+  <si>
+    <t>Province by Land Value (M. Baht)</t>
+  </si>
+  <si>
+    <t>Province by Machine Cost (M. Baht)</t>
+  </si>
+  <si>
+    <t>Province by Working Capital (M. Baht)</t>
+  </si>
+  <si>
+    <t>Province by Total Investment</t>
+  </si>
+  <si>
+    <t>จำนวนผู้ทำงานทั้งหมด</t>
+  </si>
+  <si>
+    <t>Male Workers</t>
+  </si>
+  <si>
+    <t>ผู้ทำงานชาย</t>
+  </si>
+  <si>
+    <t>Female Workers</t>
+  </si>
+  <si>
+    <t>คนงานหญิง</t>
+  </si>
+  <si>
+    <t>Province by Total Workers</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยคนงานทั้งหมด</t>
+  </si>
+  <si>
+    <t>Province by Female Workers</t>
+  </si>
+  <si>
+    <t>Province by Male Workers</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยคนงานชาย</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยคนงานหญิง</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยจำนวนโรงงาน</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยพื้นที่โรงงาน (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยพื้นที่อาคาร (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยจำนวนโรงงาน</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยพื้นที่โรงงาน (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยพื้นที่อาคาร (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยจำนวนโรงงาน</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยพื้นที่โรงงาน (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยพื้นที่อาคาร (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยจำนวนโรงงาน</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยพื้นที่โรงงาน (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยพื้นที่อาคาร (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยมูลค่าอาคาร (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยมูลค่าที่ดิน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยค่าเครื่องจักร (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยเงินทุนหมุนเวียน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยการลงทุนทั้งหมด (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยมูลค่าอาคาร (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยมูลค่าที่ดิน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยราคาเครื่อง (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยเงินทุนหมุนเวียน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยการลงทุนทั้งหมด (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยมูลค่าอาคาร (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยมูลค่าที่ดิน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยเงินทุนหมุนเวียน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยการลงทุนรวม (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยมูลค่าอาคาร (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยมูลค่าที่ดิน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยราคาเครื่องจักร (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยเงินทุนหมุนเวียน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยมูลค่าการลงทุนรวม (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยคนงานหญิง</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยคนงานทั้งหมด</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยคนงานชาย</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยคนงานหญิง</t>
+  </si>
+  <si>
+    <t>กลุ่มอุตสาหกรรมโดยจำนวนโรงงาน</t>
+  </si>
+  <si>
+    <t>กลุ่มอุตสาหกรรมโดยพื้นที่โรงงาน (ตร.ม.)</t>
+  </si>
+  <si>
+    <t>Geo_Sub_District_Chart_Title</t>
+  </si>
+  <si>
+    <t>Geo_District_Chart_Title</t>
+  </si>
+  <si>
+    <t>Wkf_Postcode_Chart_Title</t>
   </si>
 </sst>
 </file>
@@ -841,7 +943,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -859,11 +961,280 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="30">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1021,27 +1392,63 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}" name="Table1" displayName="Table1" ref="A1:D84" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="A1:D84" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}" name="Table1" displayName="Table1" ref="A1:D82" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="A1:D82" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{EA6343D5-1FE2-43FC-991F-9F660BDA0B22}" name="Entity"/>
     <tableColumn id="2" xr3:uid="{8B2E6FF6-2773-4399-9327-594910EEDC92}" name="Analysis Type"/>
-    <tableColumn id="3" xr3:uid="{23066573-0C1B-4965-95E7-7C81C836CD35}" name="English" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{58EB589B-59BD-4A1B-ACBA-F3BFBFDC54C5}" name="ภาษาไทย"/>
+    <tableColumn id="3" xr3:uid="{23066573-0C1B-4965-95E7-7C81C836CD35}" name="English" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{58EB589B-59BD-4A1B-ACBA-F3BFBFDC54C5}" name="Thai"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{316CFFA1-5176-4B66-A6A6-0F3B9A1CEC03}" name="Table2" displayName="Table2" ref="A1:C4" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{31D5C085-C5AA-4825-9DDF-4E2E1014A8F6}" name="Table4" displayName="Table4" ref="A1:C4" totalsRowShown="0" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="A1:C4" xr:uid="{31D5C085-C5AA-4825-9DDF-4E2E1014A8F6}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{59E4055D-1EF9-4081-8055-1C2379A15C98}" name="Analysis Type" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{E8C95891-C206-4014-A618-714AF2874AFC}" name="EN" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{1C7E2183-215B-4964-9102-91EA0C5981FE}" name="TH" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F6A6BB7E-8033-45E9-8A22-1F7C989FC7C9}" name="Table5" displayName="Table5" ref="A1:C6" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="A1:C6" xr:uid="{F6A6BB7E-8033-45E9-8A22-1F7C989FC7C9}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{493AAF41-4DDF-41A9-9E98-12938948A8A3}" name="Analysis Type" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{7B344CD7-2BD3-4EB6-A344-D3E72EF9E592}" name="EN" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{8EFA6C23-2809-40F4-8F83-9355E134B569}" name="TH" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{316CFFA1-5176-4B66-A6A6-0F3B9A1CEC03}" name="Table2" displayName="Table2" ref="A1:C4" totalsRowShown="0" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A1:C4" xr:uid="{316CFFA1-5176-4B66-A6A6-0F3B9A1CEC03}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{828FEEFC-73D2-498D-858C-6869171D8DFD}" name="Analysis_Type" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{5343A523-A207-4019-B160-7FABD2911CFD}" name="English" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{F4E06540-8FBF-43CA-833B-3190AFDB460B}" name="ภาษาไทย" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{828FEEFC-73D2-498D-858C-6869171D8DFD}" name="Analysis_Type" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{5343A523-A207-4019-B160-7FABD2911CFD}" name="EN" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{F4E06540-8FBF-43CA-833B-3190AFDB460B}" name="TH" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{079F0B0C-6714-45BD-971C-EE8C64A10237}" name="Table3" displayName="Table3" ref="A1:C6" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C6" xr:uid="{079F0B0C-6714-45BD-971C-EE8C64A10237}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8559CCE5-8D7A-47E2-BC30-54095AB017DE}" name="Analysis_Type" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{242DEBFA-16BE-4015-82E0-210BB57D6A46}" name="EN" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{C15480C8-3B52-499F-A23C-E49C329F1465}" name="TH" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1360,10 +1767,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B33C440-B339-49E7-80B6-40EB80459ED5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="256" zoomScaleNormal="256" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1376,21 +1783,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>171</v>
+        <v>123</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1404,7 +1811,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1418,7 +1825,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1432,7 +1839,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1446,7 +1853,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1460,21 +1867,21 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>133</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>179</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1488,7 +1895,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1530,7 +1937,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1539,1015 +1946,987 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>185</v>
+        <v>218</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>185</v>
+        <v>218</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>35</v>
+        <v>156</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>185</v>
+        <v>218</v>
       </c>
       <c r="B20">
         <v>3</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>37</v>
+        <v>160</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>185</v>
+        <v>137</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>137</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>219</v>
+      </c>
+      <c r="B24">
         <v>1</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>187</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>187</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
       <c r="C24" s="4" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>219</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>47</v>
+        <v>157</v>
       </c>
       <c r="D25" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>219</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>48</v>
+        <v>161</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
       <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D28" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29">
         <v>3</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>156</v>
-      </c>
-      <c r="B28">
+      <c r="C29" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30">
         <v>4</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>157</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>157</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
       <c r="C30" s="4" t="s">
-        <v>54</v>
+        <v>168</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>110</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>56</v>
+        <v>169</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="B32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="D32" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="B33">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>111</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>31</v>
+        <v>149</v>
       </c>
       <c r="D34" t="s">
-        <v>32</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>158</v>
+        <v>111</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>54</v>
+        <v>153</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>158</v>
+        <v>111</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>56</v>
+        <v>154</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="B38">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
       <c r="D39" t="s">
-        <v>63</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>63</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>184</v>
+        <v>112</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="D42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>184</v>
+        <v>112</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="D43" t="s">
-        <v>70</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D44" t="s">
-        <v>53</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="D45" t="s">
-        <v>72</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="D46" t="s">
-        <v>74</v>
+        <v>206</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="D47" t="s">
-        <v>76</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="B48">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>78</v>
+        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>160</v>
+        <v>113</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>79</v>
+        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>160</v>
+        <v>113</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="D50" t="s">
-        <v>81</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>160</v>
+        <v>113</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
       <c r="B52">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>84</v>
+        <v>175</v>
       </c>
       <c r="D52" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
       <c r="B53">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>86</v>
+        <v>178</v>
       </c>
       <c r="D53" t="s">
-        <v>87</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="D54" t="s">
-        <v>89</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
       <c r="B55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="D55" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
       <c r="B56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="D56" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>162</v>
+        <v>115</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="D57" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>162</v>
+        <v>220</v>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="D58" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>162</v>
+        <v>220</v>
       </c>
       <c r="B59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="D59" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>163</v>
+        <v>220</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="D60" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>116</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" t="s">
         <v>163</v>
-      </c>
-      <c r="B61">
-        <v>2</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D61" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>116</v>
+      </c>
+      <c r="B63">
         <v>3</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D62" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>164</v>
-      </c>
-      <c r="B63">
+      <c r="C63" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>117</v>
+      </c>
+      <c r="B64">
         <v>1</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D63" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>164</v>
-      </c>
-      <c r="B64">
-        <v>2</v>
-      </c>
       <c r="C64" s="4" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="D64" t="s">
-        <v>103</v>
+        <v>213</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>164</v>
+        <v>117</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="D65" t="s">
-        <v>105</v>
+        <v>214</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>165</v>
+        <v>117</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="D66" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="D67" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>110</v>
+        <v>71</v>
       </c>
       <c r="D68" t="s">
-        <v>111</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="D69" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>167</v>
+        <v>121</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="D70" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>168</v>
+        <v>121</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>116</v>
+        <v>77</v>
       </c>
       <c r="D71" t="s">
-        <v>117</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="D72" t="s">
-        <v>119</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="D73" t="s">
-        <v>121</v>
+        <v>82</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="B74">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="D74" t="s">
-        <v>123</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="B75">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="D75" t="s">
-        <v>125</v>
+        <v>216</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="B76">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="D76" t="s">
-        <v>127</v>
+        <v>217</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="D77" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="B78">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="D78" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="B79">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>132</v>
+        <v>91</v>
       </c>
       <c r="D79" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="B80">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="D80" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>170</v>
+        <v>95</v>
       </c>
       <c r="B81">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="D81" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>186</v>
+        <v>98</v>
       </c>
       <c r="B82">
         <v>0</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D82" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>140</v>
-      </c>
-      <c r="B83">
-        <v>0</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D83" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>143</v>
-      </c>
-      <c r="B84">
-        <v>0</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>145</v>
+        <v>99</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2561,11 +2940,166 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732BE711-A846-4BDE-A432-7EBD4B1436D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C297BA4-9E50-4087-B3EC-A1F48E4B6CEE}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233FB87A-43AF-450C-A59D-BA59388DC841}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732BE711-A846-4BDE-A432-7EBD4B1436D1}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2577,13 +3111,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>178</v>
+        <v>130</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2591,10 +3125,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>172</v>
+        <v>124</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>173</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2602,10 +3136,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>175</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2613,10 +3147,97 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>177</v>
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3B39290-31BF-49BD-BEDA-12EC82B25969}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All analysis pages completed except for new Home Page addition. As I want a summary page to show. I'll look at the Power BI: The art of making incredible tools for inspiration for it.
</commit_message>
<xml_diff>
--- a/Data/BiLingual Text Strings.xlsx
+++ b/Data/BiLingual Text Strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/efcfa07183130be2/Documents/001 - Power BI ^0 Data Visualisation/In Development/Active/EEC Factory Analysis - Power BI Version/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="8_{C9F57D40-F516-4FD4-9725-FDAEE5B23993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A259D03-D07D-4AFA-9A91-669F365805B0}"/>
+  <xr:revisionPtr revIDLastSave="378" documentId="8_{C9F57D40-F516-4FD4-9725-FDAEE5B23993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8633DA50-AC24-4747-A4D2-54E5A04D3BF4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" xr2:uid="{E82FD87B-5AA0-43B2-87CE-B1C55C908D64}"/>
+    <workbookView xWindow="3780" yWindow="2076" windowWidth="30960" windowHeight="12660" xr2:uid="{E82FD87B-5AA0-43B2-87CE-B1C55C908D64}"/>
   </bookViews>
   <sheets>
     <sheet name="Report Titles" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <author>tc={505AA292-25BA-43D9-8AFB-56C9758D7011}</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{337C29A6-4EC9-4AF4-BB8D-B34A3E17DC8A}">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{337C29A6-4EC9-4AF4-BB8D-B34A3E17DC8A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -59,7 +59,7 @@
     Show for all analysis Types</t>
       </text>
     </comment>
-    <comment ref="B5" authorId="1" shapeId="0" xr:uid="{47FECA0E-A023-48EA-898D-C9C2EDF509DC}">
+    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{47FECA0E-A023-48EA-898D-C9C2EDF509DC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -67,7 +67,7 @@
     Show for all analysis Types</t>
       </text>
     </comment>
-    <comment ref="B6" authorId="2" shapeId="0" xr:uid="{D312596C-DA21-4FAA-A723-D577FDCF632A}">
+    <comment ref="B8" authorId="2" shapeId="0" xr:uid="{D312596C-DA21-4FAA-A723-D577FDCF632A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -75,7 +75,7 @@
     Show for all analysis Types</t>
       </text>
     </comment>
-    <comment ref="B8" authorId="3" shapeId="0" xr:uid="{505AA292-25BA-43D9-8AFB-56C9758D7011}">
+    <comment ref="B10" authorId="3" shapeId="0" xr:uid="{505AA292-25BA-43D9-8AFB-56C9758D7011}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="226">
   <si>
     <t>Analysis Type</t>
   </si>
@@ -315,48 +315,9 @@
     <t>หญิง</t>
   </si>
   <si>
-    <t>Industry Sub-Group by No. of Factories</t>
-  </si>
-  <si>
-    <t>กลุ่มย่อยอุตสาหกรรมตามจำนวนโรงงาน</t>
-  </si>
-  <si>
-    <t>Industry Sub-Group by Factory Area (sq m.)</t>
-  </si>
-  <si>
-    <t>กลุ่มย่อยอุตสาหกรรมตามพื้นที่โรงงาน (ตร.ม.)</t>
-  </si>
-  <si>
-    <t>Industry Sub-Group by Building Area (sq m.)</t>
-  </si>
-  <si>
-    <t>กลุ่มย่อยอุตสาหกรรมตามพื้นที่อาคาร (ตร.ม.)</t>
-  </si>
-  <si>
-    <t>Industry Sub-Group by Building Value (M. Baht)</t>
-  </si>
-  <si>
-    <t>กลุ่มย่อยตามมูลค่าอาคาร (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>Industry Sub-Group by Total Workers</t>
-  </si>
-  <si>
-    <t>กลุ่มย่อยของอุตสาหกรรมโดยคนงานทั้งหมด</t>
-  </si>
-  <si>
     <t>Industry Group by No. of Factories</t>
   </si>
   <si>
-    <t>Industry Group by Factory Area (sq m.)</t>
-  </si>
-  <si>
-    <t>Industry Group by Building Area (sq m.)</t>
-  </si>
-  <si>
-    <t>กลุ่มอุตสาหกรรมจำแนกตามพื้นที่อาคาร (ตร.ม.)</t>
-  </si>
-  <si>
     <t>Industry Group by Building Value (M. Baht)</t>
   </si>
   <si>
@@ -387,9 +348,427 @@
     <t>Information_Text</t>
   </si>
   <si>
-    <t xml:space="preserve">This dashboard contains information from the Thai Government Data Playground and the information is publicly available. The dashboard retrieves the information directly from the website. I will provide the URL for the website below. I also use ISIC information from the file provided on the NSTDA website. This information is publicly available. The Industry Groups and TSIC codes might differ from sources you may already have. But I used the publicly available data. 
+    <t>English</t>
+  </si>
+  <si>
+    <t>Dashboard_Title</t>
+  </si>
+  <si>
+    <t>Province_Slicer_Title</t>
+  </si>
+  <si>
+    <t>Investment_Analysis</t>
+  </si>
+  <si>
+    <t>Workforce_Analysis</t>
+  </si>
+  <si>
+    <t>Address_details</t>
+  </si>
+  <si>
+    <t>Industry_Analysis</t>
+  </si>
+  <si>
+    <t>Geo_Province_Chart_Title</t>
+  </si>
+  <si>
+    <t>Inv_Province_Chart_Title</t>
+  </si>
+  <si>
+    <t>Inv_Total_Card_Title</t>
+  </si>
+  <si>
+    <t>Inv_District_Chart_Title</t>
+  </si>
+  <si>
+    <t>Inv_Sub-District_Chart_Title</t>
+  </si>
+  <si>
+    <t>Wkf_Province_Chart_Title</t>
+  </si>
+  <si>
+    <t>Wkf_Total_Card_Title</t>
+  </si>
+  <si>
+    <t>Wkf_District_Chart_Title</t>
+  </si>
+  <si>
+    <t>Wkf_Sub-District_Chart_Title</t>
+  </si>
+  <si>
+    <t>Wkf_Gender_Chart_Title</t>
+  </si>
+  <si>
+    <t>Wkf_Gender_Male_Legend</t>
+  </si>
+  <si>
+    <t>Wkf_Gender_Female_Legend</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>No. Of Factories</t>
+  </si>
+  <si>
+    <t>จำนวนโรงงาน</t>
+  </si>
+  <si>
+    <t>Factory Area</t>
+  </si>
+  <si>
+    <t>ขนาดพื้นที่โรงงาน</t>
+  </si>
+  <si>
+    <t>Building Area</t>
+  </si>
+  <si>
+    <t>ขนาดพื้นที่อาคาร</t>
+  </si>
+  <si>
+    <t>Analysis_Type</t>
+  </si>
+  <si>
+    <t>Analysis Types</t>
+  </si>
+  <si>
+    <t>ประเภทการวิเคราะห์</t>
+  </si>
+  <si>
+    <t>Analysis_Types_Slicer_Title</t>
+  </si>
+  <si>
+    <t>Geo_Total_Card_Title</t>
+  </si>
+  <si>
+    <t>Inv_Postcode_Chart_Title</t>
+  </si>
+  <si>
+    <t>Ind_Group_Total_Investment_Title</t>
+  </si>
+  <si>
+    <t>Geo_Postcode_Chart_Title</t>
+  </si>
+  <si>
+    <t>Thai</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>Building Value</t>
+  </si>
+  <si>
+    <t>มูลค่าอาคาร</t>
+  </si>
+  <si>
+    <t>Land Value</t>
+  </si>
+  <si>
+    <t>มูลค่าที่ดิน</t>
+  </si>
+  <si>
+    <t>Machine Cost</t>
+  </si>
+  <si>
+    <t>ค่าเครื่อง</t>
+  </si>
+  <si>
+    <t>Working Capital</t>
+  </si>
+  <si>
+    <t>เงินทุนหมุนเวียน</t>
+  </si>
+  <si>
+    <t>Total Machine Cost (M. Baht)</t>
+  </si>
+  <si>
+    <t>ค่าเครื่องจักรทั้งหมด (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>เงินทุนหมุนเวียนทั้งหมด (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>การลงทุนทั้งหมด (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>Total Working Capital (M. Baht)</t>
+  </si>
+  <si>
+    <t>Total Investment (M. Baht)</t>
+  </si>
+  <si>
+    <t>Postcode by Machine Cost (M. Baht)</t>
+  </si>
+  <si>
+    <t>Top 10 Sub-Districts by Factory Area (Sq M m.)</t>
+  </si>
+  <si>
+    <t>Top 10 Districts by Factory Area (Sq M m.)</t>
+  </si>
+  <si>
+    <t>Postcode by Factory Area (Sq M m.)</t>
+  </si>
+  <si>
+    <t>Postcode by Building Area (Sq M m.)</t>
+  </si>
+  <si>
+    <t>Top 10 Sub-Districts by Building Area (Sq M m.)</t>
+  </si>
+  <si>
+    <t>Top 10 Districts by Building Area (Sq M m.)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอแยกตามราคาเครื่อง (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอแยกคนงานทั้งหมด</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอแยกคนงานชาย</t>
+  </si>
+  <si>
+    <t>Province by Building Value (M. Baht)</t>
+  </si>
+  <si>
+    <t>Province by Land Value (M. Baht)</t>
+  </si>
+  <si>
+    <t>Province by Machine Cost (M. Baht)</t>
+  </si>
+  <si>
+    <t>Province by Working Capital (M. Baht)</t>
+  </si>
+  <si>
+    <t>Province by Total Investment</t>
+  </si>
+  <si>
+    <t>จำนวนผู้ทำงานทั้งหมด</t>
+  </si>
+  <si>
+    <t>Male Workers</t>
+  </si>
+  <si>
+    <t>ผู้ทำงานชาย</t>
+  </si>
+  <si>
+    <t>Female Workers</t>
+  </si>
+  <si>
+    <t>คนงานหญิง</t>
+  </si>
+  <si>
+    <t>Province by Total Workers</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยคนงานทั้งหมด</t>
+  </si>
+  <si>
+    <t>Province by Female Workers</t>
+  </si>
+  <si>
+    <t>Province by Male Workers</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยคนงานชาย</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยคนงานหญิง</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยจำนวนโรงงาน</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยพื้นที่โรงงาน (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยพื้นที่อาคาร (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยจำนวนโรงงาน</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยพื้นที่โรงงาน (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยพื้นที่อาคาร (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยจำนวนโรงงาน</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยพื้นที่โรงงาน (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยพื้นที่อาคาร (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยจำนวนโรงงาน</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยพื้นที่โรงงาน (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยพื้นที่อาคาร (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยมูลค่าอาคาร (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยมูลค่าที่ดิน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยค่าเครื่องจักร (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยเงินทุนหมุนเวียน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยการลงทุนทั้งหมด (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยมูลค่าอาคาร (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยมูลค่าที่ดิน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยราคาเครื่อง (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยเงินทุนหมุนเวียน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยการลงทุนทั้งหมด (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยมูลค่าอาคาร (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยมูลค่าที่ดิน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยเงินทุนหมุนเวียน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยการลงทุนรวม (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยมูลค่าอาคาร (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยมูลค่าที่ดิน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยราคาเครื่องจักร (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยเงินทุนหมุนเวียน (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยมูลค่าการลงทุนรวม (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยคนงานหญิง</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยคนงานทั้งหมด</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยคนงานชาย</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยคนงานหญิง</t>
+  </si>
+  <si>
+    <t>กลุ่มอุตสาหกรรมโดยจำนวนโรงงาน</t>
+  </si>
+  <si>
+    <t>Geo_Sub_District_Chart_Title</t>
+  </si>
+  <si>
+    <t>Geo_District_Chart_Title</t>
+  </si>
+  <si>
+    <t>Wkf_Postcode_Chart_Title</t>
+  </si>
+  <si>
+    <t>กลุ่มย่อยอุตสาหกรรมตามพื้นที่อาคาร (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>กลุ่มอุตสาหกรรมโดยพื้นที่โรงงาน (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>Industry Group by Factory Area (sq M m.)</t>
+  </si>
+  <si>
+    <t>Industry Group by Building Area (sq M m.)</t>
+  </si>
+  <si>
+    <t>กลุ่มอุตสาหกรรมจำแนกตามพื้นที่อาคาร (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>Ind_Group_Chart_Title</t>
+  </si>
+  <si>
+    <t>Ind_Sub-Category_Chart_Title</t>
+  </si>
+  <si>
+    <t>Industry Sub-Category by No. of Factories</t>
+  </si>
+  <si>
+    <t>ประเภทย่อยของอุตสาหกรรมตามจำนวนโรงงาน</t>
+  </si>
+  <si>
+    <t>Industry Sub-Category by Factory Area (sq M m.)</t>
+  </si>
+  <si>
+    <t>ประเภทย่อยของอุตสาหกรรมตามพื้นที่โรงงาน (ตร.มล.)</t>
+  </si>
+  <si>
+    <t>Industry Sub-Category by Building Area (sq M m.)</t>
+  </si>
+  <si>
+    <t>ประเภทย่อยอุตสาหกรรมตามมูลค่าอาคาร (ล้านบาท)</t>
+  </si>
+  <si>
+    <t>Industry Sub-Category by Building Value (M. Baht)</t>
+  </si>
+  <si>
+    <t>Industry Sub-Category by Total Workers</t>
+  </si>
+  <si>
+    <t>หมวดหมู่ย่อยของอุตสาหกรรมโดยผู้ปฏิบัติงานทั้งหมด</t>
+  </si>
+  <si>
+    <t>Geographic_Analysis</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>หน้าแรก</t>
+  </si>
+  <si>
+    <t>Home_Page</t>
+  </si>
+  <si>
+    <t>แดชบอร์ดนี้มีข้อมูลจาก Thai Government Data Playground และข้อมูลดังกล่าวเปิดเผยต่อสาธารณะ แดชบอร์ดดึงข้อมูลโดยตรงจากเว็บไซต์ ผมจะให้ URL สำหรับเว็บไซต์ด้านล่าง ผมยังใช้ข้อมูล ISIC จากไฟล์ที่จัดเตรียมไว้ใน สวทช. เว็บไซต์ ข้อมูลนี้เป็นข้อมูลสาธารณะ กลุ่มอุตสาหกรรมและรหัส TSIC อาจแตกต่างจากแหล่งข้อมูลที่คุณอาจมีอยู่แล้ว แต่ผมใช้ข้อมูลที่เปิดเผยต่อสาธารณะจากธนาคารแห่งประเทศไทย
+ผมใช้ข้อมูลจากวิกิพีเดียในการแปลชื่อตำบลเป็นภาษาอังกฤษ หากคุณพบปัญหาใด ๆ กับการแปล โปรดแจ้งให้เราทราบและเราจะอัปเดตตามนั้น แหล่งข้อมูลประกอบด้วยคอลัมน์ภาษาอังกฤษสำหรับคำอธิบาย ISIC (กลุ่มอุตสาหกรรม, หมวดหมู่ย่อย, TSIC)
+หากคุณประสบปัญหาในการใช้แดชบอร์ด โปรดส่งอีเมลถึงฉผมที่ datavizexpertpro@gmail.com
+Andrew Hubbard พัฒนาแดชบอร์ดนี้ในเดือนกรกฎาคม 2023
+โปรดแจ้งให้เราทราบความคิดเห็นของคุณเกี่ยวกับแดชบอร์ดและคำแนะนำสำหรับแดชบอร์ดที่ datavizexpertpro@gmail.com ผมหวังว่าจะได้รับความคิดเห็นและข้อเสนอแนะ
+แหล่งข้อมูลที่ใช้:
+ชุดข้อมูลโรงงาน: https://data.go.th/dataset/656b9ca7-10b5-4c33-87b0-188ed5fe4078/resource/b7acb5f0-e593-4437-a159-c3e761843fa8/download/eec.csv
+ชุดข้อมูล TSIC: http://pub.nstda.or.th/gov-dx/wp-content/uploads/2022/01/ISIC-BOT-Code-Rev-4-add-mark-SME_551225.xls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This dashboard contains information from the Thai Government Data Playground and the information is publicly available. The dashboard retrieves the information directly from the website. I will provide the URL for the website below. I also use ISIC information from the file provided on the NSTDA website. This information is publicly available. The Industry Groups and TSIC codes might differ from sources you may already have. But I used the publicly available data from the Bank of Thailand
 I have used information from Wikipedia to provide the English translations of Sub-district names. If you discover any issues with the translations, then please let me know and I will update them accordingly. The data source included the English language columns for ISIC descriptions (Industry Group, Sub Category, TSIC).
-If you experience problems using the Dashboard, please email at datavizexpertpro@gmail.com
+If you experience problems using the dashboard, please email me at datavizexpertpro@gmail.com
 Andrew Hubbard developed this dashboard in July 2023.
 Please let me know your comments about the dashboard and suggestions for the dashboard at datavizexpertpro@gmail.com. I look forward to receiving comments and suggestions.
 Data Sources Used:
@@ -398,374 +777,10 @@
 </t>
   </si>
   <si>
-    <t>แดชบอร์ดนี้มีข้อมูลจาก Thai Government Data Playground และข้อมูลดังกล่าวเปิดเผยต่อสาธารณะ แดชบอร์ดดึงข้อมูลโดยตรงจากเว็บไซต์ ฉันจะให้ URL สำหรับเว็บไซต์ด้านล่าง ฉันยังใช้ข้อมูล ISIC จากไฟล์ที่จัดเตรียมไว้ในเว็บไซต์ของ สวทช. ข้อมูลนี้เปิดเผยต่อสาธารณะ กลุ่มอุตสาหกรรมและรหัส TSIC อาจแตกต่างจากแหล่งที่มาที่คุณอาจมีอยู่แล้ว แต่ฉันใช้ข้อมูลที่เปิดเผยต่อสาธารณะ
-ฉันใช้ข้อมูลจากวิกิพีเดียในการแปลชื่อตำบลเป็นภาษาอังกฤษ หากคุณพบปัญหาใด ๆ กับการแปล โปรดแจ้งให้เราทราบและเราจะอัปเดตตามนั้น แหล่งข้อมูลประกอบด้วยคอลัมน์ภาษาอังกฤษสำหรับคำอธิบาย ISIC (กลุ่มอุตสาหกรรม, หมวดหมู่ย่อย, TSIC)
-หากคุณประสบปัญหาในการใช้ Dashboard โปรดส่งอีเมลมาที่ datavizexpertpro@gmail.com
-Andrew Hubbard พัฒนาแดชบอร์ดนี้ในเดือนกรกฎาคม 2023
-โปรดแจ้งให้เราทราบความคิดเห็นของคุณเกี่ยวกับแดชบอร์ดและคำแนะนำสำหรับแดชบอร์ดที่ datavizexpertpro@gmail.com ฉันหวังว่าจะได้รับความคิดเห็นและข้อเสนอแนะ
-แหล่งข้อมูลที่ใช้:
-ชุดข้อมูลโรงงาน: https://data.go.th/dataset/656b9ca7-10b5-4c33-87b0-188ed5fe4078/resource/b7acb5f0-e593-4437-a159-c3e761843fa8/download/eec.csv
-ชุดข้อมูล TSIC: http://pub.nstda.or.th/gov-dx/wp-content/uploads/2022/01/ISIC-BOT-Code-Rev-4-add-mark-SME_551225.xls</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Dashboard_Title</t>
-  </si>
-  <si>
-    <t>Province_Slicer_Title</t>
-  </si>
-  <si>
-    <t>Geographic_analysis</t>
-  </si>
-  <si>
-    <t>Investment_Analysis</t>
-  </si>
-  <si>
-    <t>Workforce_Analysis</t>
-  </si>
-  <si>
-    <t>Address_details</t>
-  </si>
-  <si>
-    <t>Industry_Analysis</t>
-  </si>
-  <si>
-    <t>Geo_Province_Chart_Title</t>
-  </si>
-  <si>
-    <t>Inv_Province_Chart_Title</t>
-  </si>
-  <si>
-    <t>Inv_Total_Card_Title</t>
-  </si>
-  <si>
-    <t>Inv_District_Chart_Title</t>
-  </si>
-  <si>
-    <t>Inv_Sub-District_Chart_Title</t>
-  </si>
-  <si>
-    <t>Wkf_Province_Chart_Title</t>
-  </si>
-  <si>
-    <t>Wkf_Total_Card_Title</t>
-  </si>
-  <si>
-    <t>Wkf_District_Chart_Title</t>
-  </si>
-  <si>
-    <t>Wkf_Sub-District_Chart_Title</t>
-  </si>
-  <si>
-    <t>Wkf_Gender_Chart_Title</t>
-  </si>
-  <si>
-    <t>Wkf_Gender_Male_Legend</t>
-  </si>
-  <si>
-    <t>Wkf_Gender_Female_Legend</t>
-  </si>
-  <si>
-    <t>Ind_Sub_Group_Analysis_Title</t>
-  </si>
-  <si>
-    <t>Ind_Group_Analysis_Title</t>
-  </si>
-  <si>
-    <t>Entity</t>
-  </si>
-  <si>
-    <t>No. Of Factories</t>
-  </si>
-  <si>
-    <t>จำนวนโรงงาน</t>
-  </si>
-  <si>
-    <t>Factory Area</t>
-  </si>
-  <si>
-    <t>ขนาดพื้นที่โรงงาน</t>
-  </si>
-  <si>
-    <t>Building Area</t>
-  </si>
-  <si>
-    <t>ขนาดพื้นที่อาคาร</t>
-  </si>
-  <si>
-    <t>Analysis_Type</t>
-  </si>
-  <si>
-    <t>Analysis Types</t>
-  </si>
-  <si>
-    <t>ประเภทการวิเคราะห์</t>
-  </si>
-  <si>
-    <t>Analysis_Types_Slicer_Title</t>
-  </si>
-  <si>
-    <t>Geo_Total_Card_Title</t>
-  </si>
-  <si>
-    <t>Inv_Postcode_Chart_Title</t>
-  </si>
-  <si>
-    <t>Ind_Group_Total_Investment_Title</t>
-  </si>
-  <si>
-    <t>Geo_Postcode_Chart_Title</t>
-  </si>
-  <si>
-    <t>Thai</t>
-  </si>
-  <si>
-    <t>EN</t>
-  </si>
-  <si>
-    <t>TH</t>
-  </si>
-  <si>
-    <t>Building Value</t>
-  </si>
-  <si>
-    <t>มูลค่าอาคาร</t>
-  </si>
-  <si>
-    <t>Land Value</t>
-  </si>
-  <si>
-    <t>มูลค่าที่ดิน</t>
-  </si>
-  <si>
-    <t>Machine Cost</t>
-  </si>
-  <si>
-    <t>ค่าเครื่อง</t>
-  </si>
-  <si>
-    <t>Working Capital</t>
-  </si>
-  <si>
-    <t>เงินทุนหมุนเวียน</t>
-  </si>
-  <si>
-    <t>Total Machine Cost (M. Baht)</t>
-  </si>
-  <si>
-    <t>ค่าเครื่องจักรทั้งหมด (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>เงินทุนหมุนเวียนทั้งหมด (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>การลงทุนทั้งหมด (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>Total Working Capital (M. Baht)</t>
-  </si>
-  <si>
-    <t>Total Investment (M. Baht)</t>
-  </si>
-  <si>
-    <t>Postcode by Machine Cost (M. Baht)</t>
-  </si>
-  <si>
-    <t>Top 10 Sub-Districts by Factory Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>Top 10 Districts by Factory Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>Postcode by Factory Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>Postcode by Building Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>Top 10 Sub-Districts by Building Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>Top 10 Districts by Building Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอแยกตามราคาเครื่อง (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอแยกคนงานทั้งหมด</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอแยกคนงานชาย</t>
-  </si>
-  <si>
-    <t>Province by Building Value (M. Baht)</t>
-  </si>
-  <si>
-    <t>Province by Land Value (M. Baht)</t>
-  </si>
-  <si>
-    <t>Province by Machine Cost (M. Baht)</t>
-  </si>
-  <si>
-    <t>Province by Working Capital (M. Baht)</t>
-  </si>
-  <si>
-    <t>Province by Total Investment</t>
-  </si>
-  <si>
-    <t>จำนวนผู้ทำงานทั้งหมด</t>
-  </si>
-  <si>
-    <t>Male Workers</t>
-  </si>
-  <si>
-    <t>ผู้ทำงานชาย</t>
-  </si>
-  <si>
-    <t>Female Workers</t>
-  </si>
-  <si>
-    <t>คนงานหญิง</t>
-  </si>
-  <si>
-    <t>Province by Total Workers</t>
-  </si>
-  <si>
-    <t>จังหวัดโดยคนงานทั้งหมด</t>
-  </si>
-  <si>
-    <t>Province by Female Workers</t>
-  </si>
-  <si>
-    <t>Province by Male Workers</t>
-  </si>
-  <si>
-    <t>จังหวัดโดยคนงานชาย</t>
-  </si>
-  <si>
-    <t>จังหวัดโดยคนงานหญิง</t>
-  </si>
-  <si>
-    <t>จังหวัดโดยจำนวนโรงงาน</t>
-  </si>
-  <si>
-    <t>จังหวัดโดยพื้นที่โรงงาน (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>จังหวัดโดยพื้นที่อาคาร (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบลโดยจำนวนโรงงาน</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบลโดยพื้นที่โรงงาน (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบลโดยพื้นที่อาคาร (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>รหัสไปรษณีย์โดยจำนวนโรงงาน</t>
-  </si>
-  <si>
-    <t>รหัสไปรษณีย์โดยพื้นที่โรงงาน (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>รหัสไปรษณีย์โดยพื้นที่อาคาร (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอโดยจำนวนโรงงาน</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอโดยพื้นที่โรงงาน (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอโดยพื้นที่อาคาร (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>จังหวัดโดยมูลค่าอาคาร (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>จังหวัดโดยมูลค่าที่ดิน (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>จังหวัดโดยค่าเครื่องจักร (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>จังหวัดโดยเงินทุนหมุนเวียน (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>จังหวัดโดยการลงทุนทั้งหมด (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>รหัสไปรษณีย์โดยมูลค่าอาคาร (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>รหัสไปรษณีย์โดยมูลค่าที่ดิน (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>รหัสไปรษณีย์โดยราคาเครื่อง (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>รหัสไปรษณีย์โดยเงินทุนหมุนเวียน (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>รหัสไปรษณีย์โดยการลงทุนทั้งหมด (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอโดยมูลค่าอาคาร (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอโดยมูลค่าที่ดิน (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอโดยเงินทุนหมุนเวียน (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอโดยการลงทุนรวม (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบลโดยมูลค่าอาคาร (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบลโดยมูลค่าที่ดิน (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบลโดยราคาเครื่องจักร (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบลโดยเงินทุนหมุนเวียน (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบลโดยมูลค่าการลงทุนรวม (ล้านบาท)</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอโดยคนงานหญิง</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบลโดยคนงานทั้งหมด</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบลโดยคนงานชาย</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบลโดยคนงานหญิง</t>
-  </si>
-  <si>
-    <t>กลุ่มอุตสาหกรรมโดยจำนวนโรงงาน</t>
-  </si>
-  <si>
-    <t>กลุ่มอุตสาหกรรมโดยพื้นที่โรงงาน (ตร.ม.)</t>
-  </si>
-  <si>
-    <t>Geo_Sub_District_Chart_Title</t>
-  </si>
-  <si>
-    <t>Geo_District_Chart_Title</t>
-  </si>
-  <si>
-    <t>Wkf_Postcode_Chart_Title</t>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>การนำทาง</t>
   </si>
 </sst>
 </file>
@@ -1392,8 +1407,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}" name="Table1" displayName="Table1" ref="A1:D82" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="A1:D82" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}" name="Table1" displayName="Table1" ref="A1:D84" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="A1:D84" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{EA6343D5-1FE2-43FC-991F-9F660BDA0B22}" name="Entity"/>
     <tableColumn id="2" xr3:uid="{8B2E6FF6-2773-4399-9327-594910EEDC92}" name="Analysis Type"/>
@@ -1749,16 +1764,16 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B4" dT="2023-07-12T02:54:24.84" personId="{34BF4BA3-CA59-44C6-848E-8B40BA430533}" id="{337C29A6-4EC9-4AF4-BB8D-B34A3E17DC8A}">
+  <threadedComment ref="B6" dT="2023-07-12T02:54:24.84" personId="{34BF4BA3-CA59-44C6-848E-8B40BA430533}" id="{337C29A6-4EC9-4AF4-BB8D-B34A3E17DC8A}">
     <text>Show for all analysis Types</text>
   </threadedComment>
-  <threadedComment ref="B5" dT="2023-07-12T02:54:33.34" personId="{34BF4BA3-CA59-44C6-848E-8B40BA430533}" id="{47FECA0E-A023-48EA-898D-C9C2EDF509DC}">
+  <threadedComment ref="B7" dT="2023-07-12T02:54:33.34" personId="{34BF4BA3-CA59-44C6-848E-8B40BA430533}" id="{47FECA0E-A023-48EA-898D-C9C2EDF509DC}">
     <text>Show for all analysis Types</text>
   </threadedComment>
-  <threadedComment ref="B6" dT="2023-07-12T02:54:39.67" personId="{34BF4BA3-CA59-44C6-848E-8B40BA430533}" id="{D312596C-DA21-4FAA-A723-D577FDCF632A}">
+  <threadedComment ref="B8" dT="2023-07-12T02:54:39.67" personId="{34BF4BA3-CA59-44C6-848E-8B40BA430533}" id="{D312596C-DA21-4FAA-A723-D577FDCF632A}">
     <text>Show for all analysis Types</text>
   </threadedComment>
-  <threadedComment ref="B8" dT="2023-07-14T08:38:54.08" personId="{34BF4BA3-CA59-44C6-848E-8B40BA430533}" id="{505AA292-25BA-43D9-8AFB-56C9758D7011}">
+  <threadedComment ref="B10" dT="2023-07-14T08:38:54.08" personId="{34BF4BA3-CA59-44C6-848E-8B40BA430533}" id="{505AA292-25BA-43D9-8AFB-56C9758D7011}">
     <text>Show for all analysis types</text>
   </threadedComment>
 </ThreadedComments>
@@ -1767,10 +1782,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B33C440-B339-49E7-80B6-40EB80459ED5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="256" zoomScaleNormal="256" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="256" zoomScaleNormal="256" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1783,21 +1798,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1811,91 +1826,88 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
+        <v>224</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>3</v>
+        <v>224</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>221</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>7</v>
+        <v>219</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>218</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>131</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1909,937 +1921,937 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14">
         <v>1</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13">
+      <c r="D14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14">
+      <c r="D15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16">
         <v>3</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>134</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19">
         <v>3</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D19" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>218</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>218</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D19" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>160</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>199</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="D21" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>199</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="D22" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>159</v>
+        <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>219</v>
+        <v>119</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>33</v>
+        <v>140</v>
       </c>
       <c r="D24" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>219</v>
+        <v>119</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="D25" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>161</v>
+        <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>200</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="D27" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>110</v>
+        <v>200</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="D28" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31">
         <v>3</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D29" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>110</v>
-      </c>
-      <c r="B30">
+      <c r="C31" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32">
         <v>4</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D30" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31">
-        <v>5</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D31" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>111</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
       <c r="C32" s="4" t="s">
-        <v>28</v>
+        <v>150</v>
       </c>
       <c r="D32" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="D33" t="s">
-        <v>36</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>149</v>
+        <v>28</v>
       </c>
       <c r="D34" t="s">
-        <v>150</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>153</v>
+        <v>35</v>
       </c>
       <c r="D35" t="s">
-        <v>151</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="D36" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="D37" t="s">
-        <v>198</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>40</v>
+        <v>136</v>
       </c>
       <c r="D38" t="s">
-        <v>199</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>155</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42">
         <v>4</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D40" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>135</v>
-      </c>
-      <c r="B41">
+      <c r="D42" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43">
         <v>5</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D41" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>112</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43">
-        <v>2</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="D43" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B44">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D44" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B45">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D45" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B46">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D46" t="s">
-        <v>206</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D47" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="B48">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B50">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D50" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53">
         <v>5</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D51" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>114</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D52" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>114</v>
-      </c>
-      <c r="B53">
-        <v>2</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>178</v>
-      </c>
       <c r="D53" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="D54" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>51</v>
+        <v>160</v>
       </c>
       <c r="D55" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>53</v>
+        <v>159</v>
       </c>
       <c r="D56" t="s">
-        <v>54</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B57">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D57" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>220</v>
+        <v>99</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D58" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>220</v>
+        <v>99</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D59" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D60" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>201</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D61" t="s">
-        <v>163</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>201</v>
       </c>
       <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>100</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>100</v>
+      </c>
+      <c r="B64">
         <v>2</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D62" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>116</v>
-      </c>
-      <c r="B63">
-        <v>3</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D63" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>117</v>
-      </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="D64" t="s">
-        <v>213</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D65" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D66" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>101</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D67" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>101</v>
+      </c>
+      <c r="B68">
         <v>3</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C68" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D66" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>118</v>
-      </c>
-      <c r="B67">
-        <v>0</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D67" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>119</v>
-      </c>
-      <c r="B68">
-        <v>0</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="D68" t="s">
-        <v>72</v>
+        <v>197</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="C69" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D69" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>103</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>104</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D71" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>121</v>
-      </c>
-      <c r="B70">
-        <v>1</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D70" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>121</v>
-      </c>
-      <c r="B71">
-        <v>2</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D71" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>121</v>
+        <v>208</v>
       </c>
       <c r="B72">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>79</v>
+        <v>209</v>
       </c>
       <c r="D72" t="s">
-        <v>80</v>
+        <v>210</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>121</v>
+        <v>208</v>
       </c>
       <c r="B73">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>81</v>
+        <v>211</v>
       </c>
       <c r="D73" t="s">
-        <v>82</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>121</v>
+        <v>208</v>
       </c>
       <c r="B74">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>83</v>
+        <v>213</v>
       </c>
       <c r="D74" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>122</v>
+        <v>208</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>85</v>
+        <v>215</v>
       </c>
       <c r="D75" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>122</v>
+        <v>208</v>
       </c>
       <c r="B76">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>86</v>
+        <v>216</v>
       </c>
       <c r="D76" t="s">
         <v>217</v>
@@ -2847,86 +2859,114 @@
     </row>
     <row r="77" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>122</v>
+        <v>207</v>
       </c>
       <c r="B77">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D77" t="s">
-        <v>88</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>122</v>
+        <v>207</v>
       </c>
       <c r="B78">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>89</v>
+        <v>204</v>
       </c>
       <c r="D78" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>122</v>
+        <v>207</v>
       </c>
       <c r="B79">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>91</v>
+        <v>205</v>
       </c>
       <c r="D79" t="s">
-        <v>92</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>136</v>
+        <v>207</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D80" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>95</v>
+        <v>207</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="D81" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="B82">
         <v>0</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>100</v>
+        <v>80</v>
+      </c>
+      <c r="D82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D83" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2958,10 +2998,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2972,7 +3012,7 @@
         <v>51</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2980,10 +3020,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2991,10 +3031,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -3024,10 +3064,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3035,10 +3075,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3046,10 +3086,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3057,10 +3097,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3068,10 +3108,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3082,7 +3122,7 @@
         <v>51</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3111,13 +3151,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3125,10 +3165,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3136,10 +3176,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3147,10 +3187,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3176,13 +3216,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3190,10 +3230,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3201,10 +3241,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3212,10 +3252,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3223,10 +3263,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed, Initial Release Version!
</commit_message>
<xml_diff>
--- a/Data/BiLingual Text Strings.xlsx
+++ b/Data/BiLingual Text Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/efcfa07183130be2/Documents/001 - Power BI ^0 Data Visualisation/In Development/Active/EEC Factory Analysis - Power BI Version/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="378" documentId="8_{C9F57D40-F516-4FD4-9725-FDAEE5B23993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8633DA50-AC24-4747-A4D2-54E5A04D3BF4}"/>
+  <xr:revisionPtr revIDLastSave="620" documentId="8_{C9F57D40-F516-4FD4-9725-FDAEE5B23993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0453597D-8D1F-4FED-A08E-9A6F6E158E34}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="2076" windowWidth="30960" windowHeight="12660" xr2:uid="{E82FD87B-5AA0-43B2-87CE-B1C55C908D64}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" xr2:uid="{E82FD87B-5AA0-43B2-87CE-B1C55C908D64}"/>
   </bookViews>
   <sheets>
     <sheet name="Report Titles" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="282">
   <si>
     <t>Analysis Type</t>
   </si>
@@ -150,30 +150,12 @@
     <t xml:space="preserve"> Province by No. of Factories</t>
   </si>
   <si>
-    <t xml:space="preserve"> Province by Factory Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>Province by Building Area (Sq M m.)</t>
-  </si>
-  <si>
     <t>Total No. of Factories</t>
   </si>
   <si>
     <t>จำนวนโรงงานทั้งหมด</t>
   </si>
   <si>
-    <t>Total Factory Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>พื้นที่โรงงานทั้งหมด (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>Total Building Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>พื้นที่อาคารทั้งหมด (ตร.มล.)</t>
-  </si>
-  <si>
     <t>Total Building Value (M. Baht)</t>
   </si>
   <si>
@@ -504,24 +486,6 @@
     <t>Postcode by Machine Cost (M. Baht)</t>
   </si>
   <si>
-    <t>Top 10 Sub-Districts by Factory Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>Top 10 Districts by Factory Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>Postcode by Factory Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>Postcode by Building Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>Top 10 Sub-Districts by Building Area (Sq M m.)</t>
-  </si>
-  <si>
-    <t>Top 10 Districts by Building Area (Sq M m.)</t>
-  </si>
-  <si>
     <t>10 อันดับอำเภอแยกตามราคาเครื่อง (ล้านบาท)</t>
   </si>
   <si>
@@ -582,39 +546,15 @@
     <t>จังหวัดโดยจำนวนโรงงาน</t>
   </si>
   <si>
-    <t>จังหวัดโดยพื้นที่โรงงาน (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>จังหวัดโดยพื้นที่อาคาร (ตร.มล.)</t>
-  </si>
-  <si>
     <t>10 อันดับตำบลโดยจำนวนโรงงาน</t>
   </si>
   <si>
-    <t>10 อันดับตำบลโดยพื้นที่โรงงาน (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>10 อันดับตำบลโดยพื้นที่อาคาร (ตร.มล.)</t>
-  </si>
-  <si>
     <t>รหัสไปรษณีย์โดยจำนวนโรงงาน</t>
   </si>
   <si>
-    <t>รหัสไปรษณีย์โดยพื้นที่โรงงาน (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>รหัสไปรษณีย์โดยพื้นที่อาคาร (ตร.มล.)</t>
-  </si>
-  <si>
     <t>10 อันดับอำเภอโดยจำนวนโรงงาน</t>
   </si>
   <si>
-    <t>10 อันดับอำเภอโดยพื้นที่โรงงาน (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>10 อันดับอำเภอโดยพื้นที่อาคาร (ตร.มล.)</t>
-  </si>
-  <si>
     <t>จังหวัดโดยมูลค่าอาคาร (ล้านบาท)</t>
   </si>
   <si>
@@ -699,18 +639,6 @@
     <t>กลุ่มย่อยอุตสาหกรรมตามพื้นที่อาคาร (ตร.มล.)</t>
   </si>
   <si>
-    <t>กลุ่มอุตสาหกรรมโดยพื้นที่โรงงาน (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>Industry Group by Factory Area (sq M m.)</t>
-  </si>
-  <si>
-    <t>Industry Group by Building Area (sq M m.)</t>
-  </si>
-  <si>
-    <t>กลุ่มอุตสาหกรรมจำแนกตามพื้นที่อาคาร (ตร.มล.)</t>
-  </si>
-  <si>
     <t>Ind_Group_Chart_Title</t>
   </si>
   <si>
@@ -721,15 +649,6 @@
   </si>
   <si>
     <t>ประเภทย่อยของอุตสาหกรรมตามจำนวนโรงงาน</t>
-  </si>
-  <si>
-    <t>Industry Sub-Category by Factory Area (sq M m.)</t>
-  </si>
-  <si>
-    <t>ประเภทย่อยของอุตสาหกรรมตามพื้นที่โรงงาน (ตร.มล.)</t>
-  </si>
-  <si>
-    <t>Industry Sub-Category by Building Area (sq M m.)</t>
   </si>
   <si>
     <t>ประเภทย่อยอุตสาหกรรมตามมูลค่าอาคาร (ล้านบาท)</t>
@@ -782,12 +701,261 @@
   <si>
     <t>การนำทาง</t>
   </si>
+  <si>
+    <t>Home_Total_Factories</t>
+  </si>
+  <si>
+    <t>Home_Total_Industry_Groups</t>
+  </si>
+  <si>
+    <t>Home_Total_Districts</t>
+  </si>
+  <si>
+    <t>Home_Total_Sub-Districts</t>
+  </si>
+  <si>
+    <t>การนับกลุ่มอุตสาหกรรม</t>
+  </si>
+  <si>
+    <t>Industry Group Count</t>
+  </si>
+  <si>
+    <t>Factory District Reach</t>
+  </si>
+  <si>
+    <t>โรงงานตำบลเข้าถึง</t>
+  </si>
+  <si>
+    <t>การเข้าถึงอำเภอโรงงาน</t>
+  </si>
+  <si>
+    <t>Home_Factory_Area</t>
+  </si>
+  <si>
+    <t>Home_Building_Area</t>
+  </si>
+  <si>
+    <t>Industry Sub-Category by Building Area (sq Mm.)</t>
+  </si>
+  <si>
+    <t>Home_Page_Navigation_Tooltip</t>
+  </si>
+  <si>
+    <t>Geographic_Navigation_Tooltip</t>
+  </si>
+  <si>
+    <t>Investment_Navigation_Tooltip</t>
+  </si>
+  <si>
+    <t>Workforce_Navigation_Tooltip</t>
+  </si>
+  <si>
+    <t>Industry_Navigation_Tooltip</t>
+  </si>
+  <si>
+    <t>Address_Navigation_Tooltip</t>
+  </si>
+  <si>
+    <t>Information_Navigation_Tooltip</t>
+  </si>
+  <si>
+    <t>Click here to navigate to the Industry Dashboard</t>
+  </si>
+  <si>
+    <t>Click here to navigate to the Information Page</t>
+  </si>
+  <si>
+    <t>Click here to go to the Home Page.</t>
+  </si>
+  <si>
+    <t>คลิกที่นี่เพื่อไปที่หน้าแรก</t>
+  </si>
+  <si>
+    <t>Click here to go to the Geographic Dashboard</t>
+  </si>
+  <si>
+    <t>คลิกที่นี่เพื่อไปที่แดชบอร์ดทางภูมิศาสตร์</t>
+  </si>
+  <si>
+    <t>Click here to go to the Investment Dashboard</t>
+  </si>
+  <si>
+    <t>คลิกที่นี่เพื่อนำทางไปยังอุตสาหกรรม</t>
+  </si>
+  <si>
+    <t>คลิกที่นี่เพื่อไปที่แดชบอร์ดการลงทุน</t>
+  </si>
+  <si>
+    <t>คลิกที่นี่เพื่อไปที่แดชบอร์ดพนักงาน</t>
+  </si>
+  <si>
+    <t>Click here to go to the Address Details page</t>
+  </si>
+  <si>
+    <t>คลิกที่นี่เพื่อไปที่หน้ารายละเอียดที่อยู่</t>
+  </si>
+  <si>
+    <t>คลิกที่นี่เพื่อไปยังหน้าข้อมูล</t>
+  </si>
+  <si>
+    <t>Factory Sub-Dist. Reach</t>
+  </si>
+  <si>
+    <t>Factory Area (Sq km)</t>
+  </si>
+  <si>
+    <t>พื้นที่โรงงาน  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>พื้นที่อาคาร  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>Building Area (Sq km)</t>
+  </si>
+  <si>
+    <t>กลุ่มอุตสาหกรรมจำแนกตามพื้นที่อาคาร  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>Industry Group by Building Area (sq km)</t>
+  </si>
+  <si>
+    <t>Industry Group by Factory Area (sq km)</t>
+  </si>
+  <si>
+    <t>กลุ่มอุตสาหกรรมโดยพื้นที่โรงงาน  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>Industry Sub-Category by Factory Area (sq km.)</t>
+  </si>
+  <si>
+    <t>ประเภทย่อยของอุตสาหกรรมตามพื้นที่โรงงาน  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยพื้นที่อาคาร  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>10 อันดับอำเภอโดยพื้นที่โรงงาน  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>Top 10 Districts by Building Area (Sq km)</t>
+  </si>
+  <si>
+    <t>Top 10 Districts by Factory Area (Sq km)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยพื้นที่อาคาร   (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>รหัสไปรษณีย์โดยพื้นที่โรงงาน  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยพื้นที่อาคาร  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>Top 10 Sub-Districts by Building Area (Sq km)</t>
+  </si>
+  <si>
+    <t>Postcode by Factory Area (Sq km)</t>
+  </si>
+  <si>
+    <t>Postcode by Building Area (Sq km)</t>
+  </si>
+  <si>
+    <t>Top 10 Sub-Districts by Factory Area (Sq km)</t>
+  </si>
+  <si>
+    <t>10 อันดับตำบลโดยพื้นที่โรงงาน  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>Total Building Area (Sq km)</t>
+  </si>
+  <si>
+    <t>พื้นที่อาคารทั้งหมด  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>Total Factory Area (Sq km)</t>
+  </si>
+  <si>
+    <t>พื้นที่โรงงานทั้งหมด  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>Province by Building Area (Sq km)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยพื้นที่อาคาร  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t>จังหวัดโดยพื้นที่โรงงาน  (ตร.กม.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Province by Factory Area (Sq km)</t>
+  </si>
+  <si>
+    <t>Home_Total_Workers</t>
+  </si>
+  <si>
+    <t>Home_Area_Of_Coverage</t>
+  </si>
+  <si>
+    <t>Eastern Economic Corridor Report Coverage Area</t>
+  </si>
+  <si>
+    <t>พื้นที่รายงานระเบียงเศรษฐกิจพิเศษภาคตะวันออก</t>
+  </si>
+  <si>
+    <t>Click here to go to the Workforce Dashboard</t>
+  </si>
+  <si>
+    <t>Home_Page_Title</t>
+  </si>
+  <si>
+    <t>Eastern Economic Corridor Report Home Page</t>
+  </si>
+  <si>
+    <t>หน้าแรกรายงานระเบียงเศรษฐกิจพิเศษภาคตะวันออก</t>
+  </si>
+  <si>
+    <t>Click here to change report language to English</t>
+  </si>
+  <si>
+    <t>คลิกที่นี่เพื่อเปลี่ยนภาษารายงานเป็นภาษาไทย</t>
+  </si>
+  <si>
+    <t>Language_Buttons_Tooltip</t>
+  </si>
+  <si>
+    <t>Click this button to rest all the slicers on this page to default settings</t>
+  </si>
+  <si>
+    <t>คลิกปุ่มนี้เพื่อพักตัวแบ่งส่วนข้อมูลทั้งหมดในหน้านี้เป็นการตั้งค่าเริ่มต้น</t>
+  </si>
+  <si>
+    <t>Clear_Slicers_Button_Tooltip</t>
+  </si>
+  <si>
+    <t>Address_District_Slicer_Title</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>อำเภอ</t>
+  </si>
+  <si>
+    <t>Address_Sub-District_Slicer_Title</t>
+  </si>
+  <si>
+    <t>Sub-District</t>
+  </si>
+  <si>
+    <t>ตำบล</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -810,6 +978,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -958,7 +1137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -977,6 +1156,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1407,8 +1588,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}" name="Table1" displayName="Table1" ref="A1:D84" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="A1:D84" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}" name="Table1" displayName="Table1" ref="A1:D104" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="A1:D104" xr:uid="{0917F25E-D7BC-4107-A6D7-711E76F41266}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{EA6343D5-1FE2-43FC-991F-9F660BDA0B22}" name="Entity"/>
     <tableColumn id="2" xr3:uid="{8B2E6FF6-2773-4399-9327-594910EEDC92}" name="Analysis Type"/>
@@ -1782,37 +1963,37 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B33C440-B339-49E7-80B6-40EB80459ED5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="256" zoomScaleNormal="256" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B98" zoomScale="256" zoomScaleNormal="256" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.6640625" customWidth="1"/>
     <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="51.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1826,18 +2007,18 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1851,21 +2032,21 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="D5" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>191</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1879,7 +2060,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1893,7 +2074,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1907,7 +2088,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1921,7 +2102,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1949,16 +2130,16 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D12" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1977,7 +2158,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1986,987 +2167,1267 @@
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>20</v>
+        <v>261</v>
       </c>
       <c r="D15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>21</v>
+        <v>258</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>24</v>
+        <v>256</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>26</v>
+        <v>254</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>138</v>
+        <v>252</v>
       </c>
       <c r="D21" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>142</v>
+        <v>249</v>
       </c>
       <c r="D22" t="s">
-        <v>168</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>140</v>
+        <v>250</v>
       </c>
       <c r="D24" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B25">
         <v>3</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>141</v>
+        <v>251</v>
       </c>
       <c r="D25" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>139</v>
+        <v>245</v>
       </c>
       <c r="D27" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>143</v>
+        <v>244</v>
       </c>
       <c r="D28" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D29" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B31">
         <v>3</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D31" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="D32" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B33">
         <v>5</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="D33" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D35" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B37">
         <v>4</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D37" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B38">
         <v>5</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D38" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B40">
         <v>2</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D40" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B41">
         <v>3</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D41" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B42">
         <v>4</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D42" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B43">
         <v>5</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D43" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D44" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B45">
         <v>2</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D45" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B46">
         <v>3</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D46" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B47">
         <v>4</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D47" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B48">
         <v>5</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D48" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D49" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B50">
         <v>2</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D50" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B51">
         <v>3</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D51" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B52">
         <v>4</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D52" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B53">
         <v>5</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D53" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D54" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B55">
         <v>2</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="D55" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B56">
         <v>3</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D56" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D57" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B58">
         <v>2</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D58" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B59">
         <v>3</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D59" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D60" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B61">
         <v>2</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D61" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B62">
         <v>3</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D62" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D63" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B64">
         <v>2</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D64" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B65">
         <v>3</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D65" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D66" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B67">
         <v>2</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D67" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B68">
         <v>3</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D68" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D69" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D70" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D71" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="B72">
         <v>1</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D72" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="B73">
         <v>2</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="D73" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="B74">
         <v>3</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D74" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="B75">
         <v>4</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="D75" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="B76">
         <v>5</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="D76" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="B77">
         <v>1</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D77" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="B78">
         <v>2</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>204</v>
+        <v>238</v>
       </c>
       <c r="D78" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="B79">
         <v>3</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>205</v>
+        <v>237</v>
       </c>
       <c r="D79" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="B80">
         <v>4</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D80" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="B81">
         <v>5</v>
       </c>
       <c r="C81" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D81" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>112</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D82" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>76</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D83" t="s">
         <v>78</v>
-      </c>
-      <c r="D81" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>118</v>
-      </c>
-      <c r="B82">
-        <v>0</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D82" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>82</v>
-      </c>
-      <c r="B83">
-        <v>0</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D83" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B84">
         <v>0</v>
       </c>
       <c r="C84" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>199</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D85" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>200</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>201</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D87" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>202</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D88" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>208</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D89" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>209</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D90" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>262</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D91" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>263</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D92" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>267</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D93" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>211</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>212</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D95" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="D84" s="4" t="s">
-        <v>222</v>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>213</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>214</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>215</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>216</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>217</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>272</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>275</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>276</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D103" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>279</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D104" s="14" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -2998,10 +3459,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3009,10 +3470,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3020,10 +3481,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3031,10 +3492,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3064,10 +3525,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3075,10 +3536,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3086,10 +3547,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3097,10 +3558,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3108,10 +3569,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3119,10 +3580,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3151,13 +3612,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3165,10 +3626,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3176,10 +3637,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3187,10 +3648,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -3216,13 +3677,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3230,10 +3691,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3241,10 +3702,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3252,10 +3713,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3263,10 +3724,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3274,10 +3735,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>